<commit_message>
Update Failure Mode Analysis.xlsx
</commit_message>
<xml_diff>
--- a/Failure Mode Analysis.xlsx
+++ b/Failure Mode Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop\Documents\GitHub\L2-DESIGN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F26F39DF-497A-4180-8AA1-942126CD63D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859CB5DB-1F9B-45FC-94EF-FC79CCB4ABE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D1A17FD6-6A2B-4E61-81B2-FDB88576B0B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D1A17FD6-6A2B-4E61-81B2-FDB88576B0B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,27 +60,18 @@
     <t>Liklihood?</t>
   </si>
   <si>
-    <t>Hard Casing, anti vibration (metal fatigue/work hardening)</t>
-  </si>
-  <si>
     <t>Over Charging</t>
   </si>
   <si>
     <t>Decreased Capacity, fire, explosion, expansion due to c02</t>
   </si>
   <si>
-    <t>Smart Charger, detailed user manual, battery health monitor</t>
-  </si>
-  <si>
     <t>Over Discharge</t>
   </si>
   <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>Anti-short connectors, idle mode, battery monitor, hibernation, isolation switch</t>
-  </si>
-  <si>
     <t>Terminal Short</t>
   </si>
   <si>
@@ -120,21 +111,12 @@
     <t>Rate the coin battery to sufficient capacity</t>
   </si>
   <si>
-    <t>FETs failing into a short</t>
-  </si>
-  <si>
-    <t>Fets failing into an open</t>
-  </si>
-  <si>
     <t>No Effect, As is the system is in idle mode</t>
   </si>
   <si>
     <t>Falls through to idle Mode, battery pack is isolated</t>
   </si>
   <si>
-    <t>HOW TO DETECT?</t>
-  </si>
-  <si>
     <t>Current or Voltage Sensor Fails</t>
   </si>
   <si>
@@ -144,9 +126,6 @@
     <t>If only one of the two sensors is borken, there must be an error, go into exception state, error codes.</t>
   </si>
   <si>
-    <t>Arduino</t>
-  </si>
-  <si>
     <t>No voltage appears on analogue inputs</t>
   </si>
   <si>
@@ -247,6 +226,27 @@
   </si>
   <si>
     <t>Ensure proper airflow to the heatsinks</t>
+  </si>
+  <si>
+    <t>Fuses, Hard Casing, anti vibration (metal fatigue/work hardening)</t>
+  </si>
+  <si>
+    <t>Fuses, Smart Charger, detailed user manual, battery health monitor</t>
+  </si>
+  <si>
+    <t>Fuses, Anti-short connectors, idle mode, battery monitor, hibernation, isolation switch</t>
+  </si>
+  <si>
+    <t>Load Switches failing into a short</t>
+  </si>
+  <si>
+    <t>Load Switches failing into an open</t>
+  </si>
+  <si>
+    <t>Detect a lack of heartbeat appearing from microcontroller, throw error</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
   </si>
 </sst>
 </file>
@@ -528,81 +528,128 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,428 +967,428 @@
   <dimension ref="B1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
-    <col min="4" max="4" width="108.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" customWidth="1"/>
-    <col min="7" max="7" width="73.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="57.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="48.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="27"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="28" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="11" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="29"/>
+    </row>
+    <row r="4" spans="2:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="25"/>
-    </row>
-    <row r="4" spans="2:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="12" t="s">
+    </row>
+    <row r="8" spans="2:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="G8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="12" t="s">
+    </row>
+    <row r="9" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="22"/>
+      <c r="C9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="26" t="s">
+      <c r="G9" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="22"/>
+      <c r="C10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="22"/>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="36" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="32" t="s">
+      <c r="F11" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="23"/>
+      <c r="C12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="38"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="22"/>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="22"/>
+      <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="22"/>
+      <c r="C16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="22"/>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="22"/>
+      <c r="C18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="23"/>
+      <c r="C19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="22"/>
+      <c r="C21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="22"/>
+      <c r="C22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="22"/>
+      <c r="C23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="33" t="s">
+      <c r="G23" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="23"/>
+      <c r="C24" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="5"/>
-      <c r="C12" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="4"/>
-      <c r="C16" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
-      <c r="C17" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="4"/>
-      <c r="C18" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="5"/>
-      <c r="C19" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="4"/>
-      <c r="C21" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="4"/>
-      <c r="C22" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="15" t="s">
+      <c r="G24" s="9" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="4"/>
-      <c r="C23" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="5"/>
-      <c r="C24" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>